<commit_message>
Upload Y4_B2526_General_Surgery_checklist1758135318655_backup@backdoor.com.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_General_Surgery_checklist1758135318655_backup@backdoor.com.xlsx
+++ b/log_history/Y4_B2526_General_Surgery_checklist1758135318655_backup@backdoor.com.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\Imported_logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\log_history\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66252A40-9757-4FF8-99FA-BC3034872CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D07A85E-96C7-4941-8AED-7A67020D7A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="1300" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1300" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Checklist" sheetId="1" r:id="rId1"/>
@@ -333,13 +333,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="168" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -365,10 +372,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,17 +719,17 @@
   <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D2" sqref="D2:D93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="14.08203125" customWidth="1"/>
     <col min="3" max="3" width="10.25" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -741,7 +749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -751,8 +759,8 @@
       <c r="C2" s="1">
         <v>45911</v>
       </c>
-      <c r="D2" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D2" s="3">
+        <v>0.46059027777777778</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -761,7 +769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -771,8 +779,8 @@
       <c r="C3" s="1">
         <v>45911</v>
       </c>
-      <c r="D3" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D3" s="3">
+        <v>0.46059027777777778</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -781,7 +789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -791,8 +799,8 @@
       <c r="C4" s="1">
         <v>45911</v>
       </c>
-      <c r="D4" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D4" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
@@ -801,7 +809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -811,8 +819,8 @@
       <c r="C5" s="1">
         <v>45911</v>
       </c>
-      <c r="D5" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D5" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -821,7 +829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -831,8 +839,8 @@
       <c r="C6" s="1">
         <v>45911</v>
       </c>
-      <c r="D6" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D6" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -841,7 +849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -851,8 +859,8 @@
       <c r="C7" s="1">
         <v>45911</v>
       </c>
-      <c r="D7" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D7" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -861,7 +869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -871,8 +879,8 @@
       <c r="C8" s="1">
         <v>45911</v>
       </c>
-      <c r="D8" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D8" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -881,7 +889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -891,8 +899,8 @@
       <c r="C9" s="1">
         <v>45911</v>
       </c>
-      <c r="D9" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D9" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -901,7 +909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -911,8 +919,8 @@
       <c r="C10" s="1">
         <v>45911</v>
       </c>
-      <c r="D10" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D10" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -921,7 +929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -931,8 +939,8 @@
       <c r="C11" s="1">
         <v>45911</v>
       </c>
-      <c r="D11" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D11" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -941,7 +949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -951,8 +959,8 @@
       <c r="C12" s="1">
         <v>45911</v>
       </c>
-      <c r="D12" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D12" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -961,7 +969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -971,8 +979,8 @@
       <c r="C13" s="1">
         <v>45911</v>
       </c>
-      <c r="D13" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D13" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -981,7 +989,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -991,8 +999,8 @@
       <c r="C14" s="1">
         <v>45911</v>
       </c>
-      <c r="D14" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D14" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1001,7 +1009,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1011,8 +1019,8 @@
       <c r="C15" s="1">
         <v>45911</v>
       </c>
-      <c r="D15" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D15" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1021,7 +1029,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1031,8 +1039,8 @@
       <c r="C16" s="1">
         <v>45911</v>
       </c>
-      <c r="D16" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D16" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -1041,7 +1049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1051,8 +1059,8 @@
       <c r="C17" s="1">
         <v>45911</v>
       </c>
-      <c r="D17" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D17" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
@@ -1061,7 +1069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1071,8 +1079,8 @@
       <c r="C18" s="1">
         <v>45911</v>
       </c>
-      <c r="D18" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D18" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1081,7 +1089,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1091,8 +1099,8 @@
       <c r="C19" s="1">
         <v>45911</v>
       </c>
-      <c r="D19" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D19" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -1101,7 +1109,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1111,8 +1119,8 @@
       <c r="C20" s="1">
         <v>45911</v>
       </c>
-      <c r="D20" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D20" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
@@ -1121,7 +1129,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1131,8 +1139,8 @@
       <c r="C21" s="1">
         <v>45911</v>
       </c>
-      <c r="D21" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D21" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -1141,7 +1149,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1151,8 +1159,8 @@
       <c r="C22" s="1">
         <v>45911</v>
       </c>
-      <c r="D22" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D22" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -1161,7 +1169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1171,8 +1179,8 @@
       <c r="C23" s="1">
         <v>45911</v>
       </c>
-      <c r="D23" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D23" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -1181,7 +1189,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1191,8 +1199,8 @@
       <c r="C24" s="1">
         <v>45911</v>
       </c>
-      <c r="D24" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D24" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -1201,7 +1209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1211,8 +1219,8 @@
       <c r="C25" s="1">
         <v>45911</v>
       </c>
-      <c r="D25" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D25" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -1221,7 +1229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1231,8 +1239,8 @@
       <c r="C26" s="1">
         <v>45911</v>
       </c>
-      <c r="D26" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D26" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E26" t="s">
         <v>8</v>
@@ -1241,7 +1249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1251,8 +1259,8 @@
       <c r="C27" s="1">
         <v>45911</v>
       </c>
-      <c r="D27" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D27" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E27" t="s">
         <v>8</v>
@@ -1261,7 +1269,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1271,8 +1279,8 @@
       <c r="C28" s="1">
         <v>45911</v>
       </c>
-      <c r="D28" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D28" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
@@ -1281,7 +1289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1291,8 +1299,8 @@
       <c r="C29" s="1">
         <v>45911</v>
       </c>
-      <c r="D29" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D29" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
@@ -1301,7 +1309,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1311,8 +1319,8 @@
       <c r="C30" s="1">
         <v>45911</v>
       </c>
-      <c r="D30" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D30" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -1321,7 +1329,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1331,8 +1339,8 @@
       <c r="C31" s="1">
         <v>45911</v>
       </c>
-      <c r="D31" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D31" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -1341,7 +1349,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -1351,8 +1359,8 @@
       <c r="C32" s="1">
         <v>45911</v>
       </c>
-      <c r="D32" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D32" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E32" t="s">
         <v>8</v>
@@ -1361,7 +1369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1371,8 +1379,8 @@
       <c r="C33" s="1">
         <v>45911</v>
       </c>
-      <c r="D33" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D33" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>
@@ -1381,7 +1389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -1391,8 +1399,8 @@
       <c r="C34" s="1">
         <v>45911</v>
       </c>
-      <c r="D34" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D34" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
@@ -1401,7 +1409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -1411,8 +1419,8 @@
       <c r="C35" s="1">
         <v>45911</v>
       </c>
-      <c r="D35" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D35" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -1421,7 +1429,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -1431,8 +1439,8 @@
       <c r="C36" s="1">
         <v>45911</v>
       </c>
-      <c r="D36" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D36" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E36" t="s">
         <v>8</v>
@@ -1441,7 +1449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -1451,8 +1459,8 @@
       <c r="C37" s="1">
         <v>45911</v>
       </c>
-      <c r="D37" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D37" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E37" t="s">
         <v>8</v>
@@ -1461,7 +1469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -1471,8 +1479,8 @@
       <c r="C38" s="1">
         <v>45911</v>
       </c>
-      <c r="D38" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D38" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E38" t="s">
         <v>8</v>
@@ -1481,7 +1489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -1491,8 +1499,8 @@
       <c r="C39" s="1">
         <v>45911</v>
       </c>
-      <c r="D39" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D39" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E39" t="s">
         <v>8</v>
@@ -1501,7 +1509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -1511,8 +1519,8 @@
       <c r="C40" s="1">
         <v>45911</v>
       </c>
-      <c r="D40" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D40" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E40" t="s">
         <v>8</v>
@@ -1521,7 +1529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1531,8 +1539,8 @@
       <c r="C41" s="1">
         <v>45911</v>
       </c>
-      <c r="D41" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D41" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E41" t="s">
         <v>8</v>
@@ -1541,7 +1549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -1551,8 +1559,8 @@
       <c r="C42" s="1">
         <v>45911</v>
       </c>
-      <c r="D42" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D42" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E42" t="s">
         <v>8</v>
@@ -1561,7 +1569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -1571,8 +1579,8 @@
       <c r="C43" s="1">
         <v>45911</v>
       </c>
-      <c r="D43" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D43" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -1581,7 +1589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1591,8 +1599,8 @@
       <c r="C44" s="1">
         <v>45911</v>
       </c>
-      <c r="D44" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D44" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -1601,7 +1609,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -1611,8 +1619,8 @@
       <c r="C45" s="1">
         <v>45911</v>
       </c>
-      <c r="D45" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D45" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -1621,7 +1629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -1631,8 +1639,8 @@
       <c r="C46" s="1">
         <v>45911</v>
       </c>
-      <c r="D46" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D46" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E46" t="s">
         <v>8</v>
@@ -1641,7 +1649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -1651,8 +1659,8 @@
       <c r="C47" s="1">
         <v>45911</v>
       </c>
-      <c r="D47" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D47" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E47" t="s">
         <v>8</v>
@@ -1661,7 +1669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -1671,8 +1679,8 @@
       <c r="C48" s="1">
         <v>45911</v>
       </c>
-      <c r="D48" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D48" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
@@ -1681,7 +1689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -1691,8 +1699,8 @@
       <c r="C49" s="1">
         <v>45911</v>
       </c>
-      <c r="D49" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D49" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E49" t="s">
         <v>8</v>
@@ -1701,7 +1709,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1711,8 +1719,8 @@
       <c r="C50" s="1">
         <v>45911</v>
       </c>
-      <c r="D50" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D50" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E50" t="s">
         <v>8</v>
@@ -1721,7 +1729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -1731,8 +1739,8 @@
       <c r="C51" s="1">
         <v>45911</v>
       </c>
-      <c r="D51" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D51" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E51" t="s">
         <v>8</v>
@@ -1741,7 +1749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -1751,8 +1759,8 @@
       <c r="C52" s="1">
         <v>45911</v>
       </c>
-      <c r="D52" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D52" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E52" t="s">
         <v>8</v>
@@ -1761,7 +1769,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -1771,8 +1779,8 @@
       <c r="C53" s="1">
         <v>45911</v>
       </c>
-      <c r="D53" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D53" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E53" t="s">
         <v>8</v>
@@ -1781,7 +1789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -1791,8 +1799,8 @@
       <c r="C54" s="1">
         <v>45911</v>
       </c>
-      <c r="D54" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D54" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E54" t="s">
         <v>8</v>
@@ -1801,7 +1809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -1811,8 +1819,8 @@
       <c r="C55" s="1">
         <v>45911</v>
       </c>
-      <c r="D55" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D55" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E55" t="s">
         <v>8</v>
@@ -1821,7 +1829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -1831,8 +1839,8 @@
       <c r="C56" s="1">
         <v>45911</v>
       </c>
-      <c r="D56" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D56" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E56" t="s">
         <v>8</v>
@@ -1841,7 +1849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -1851,8 +1859,8 @@
       <c r="C57" s="1">
         <v>45911</v>
       </c>
-      <c r="D57" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D57" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E57" t="s">
         <v>8</v>
@@ -1861,7 +1869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -1871,8 +1879,8 @@
       <c r="C58" s="1">
         <v>45911</v>
       </c>
-      <c r="D58" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D58" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E58" t="s">
         <v>8</v>
@@ -1881,7 +1889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -1891,8 +1899,8 @@
       <c r="C59" s="1">
         <v>45911</v>
       </c>
-      <c r="D59" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D59" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E59" t="s">
         <v>8</v>
@@ -1901,7 +1909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -1911,8 +1919,8 @@
       <c r="C60" s="1">
         <v>45911</v>
       </c>
-      <c r="D60" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D60" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E60" t="s">
         <v>8</v>
@@ -1921,7 +1929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -1931,8 +1939,8 @@
       <c r="C61" s="1">
         <v>45911</v>
       </c>
-      <c r="D61" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D61" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E61" t="s">
         <v>8</v>
@@ -1941,7 +1949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -1951,8 +1959,8 @@
       <c r="C62" s="1">
         <v>45911</v>
       </c>
-      <c r="D62" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D62" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E62" t="s">
         <v>12</v>
@@ -1961,7 +1969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -1971,8 +1979,8 @@
       <c r="C63" s="1">
         <v>45911</v>
       </c>
-      <c r="D63" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D63" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E63" t="s">
         <v>8</v>
@@ -1981,7 +1989,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -1991,8 +1999,8 @@
       <c r="C64" s="1">
         <v>45911</v>
       </c>
-      <c r="D64" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D64" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E64" t="s">
         <v>12</v>
@@ -2001,7 +2009,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -2011,8 +2019,8 @@
       <c r="C65" s="1">
         <v>45911</v>
       </c>
-      <c r="D65" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D65" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E65" t="s">
         <v>12</v>
@@ -2021,7 +2029,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -2031,8 +2039,8 @@
       <c r="C66" s="1">
         <v>45911</v>
       </c>
-      <c r="D66" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D66" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E66" t="s">
         <v>8</v>
@@ -2041,7 +2049,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -2051,8 +2059,8 @@
       <c r="C67" s="1">
         <v>45911</v>
       </c>
-      <c r="D67" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D67" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E67" t="s">
         <v>8</v>
@@ -2061,7 +2069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -2071,8 +2079,8 @@
       <c r="C68" s="1">
         <v>45911</v>
       </c>
-      <c r="D68" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D68" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E68" t="s">
         <v>8</v>
@@ -2081,7 +2089,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -2091,8 +2099,8 @@
       <c r="C69" s="1">
         <v>45911</v>
       </c>
-      <c r="D69" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D69" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E69" t="s">
         <v>8</v>
@@ -2101,7 +2109,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>78</v>
       </c>
@@ -2111,8 +2119,8 @@
       <c r="C70" s="1">
         <v>45911</v>
       </c>
-      <c r="D70" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D70" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E70" t="s">
         <v>8</v>
@@ -2121,7 +2129,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -2131,8 +2139,8 @@
       <c r="C71" s="1">
         <v>45911</v>
       </c>
-      <c r="D71" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D71" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E71" t="s">
         <v>12</v>
@@ -2141,7 +2149,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -2151,8 +2159,8 @@
       <c r="C72" s="1">
         <v>45911</v>
       </c>
-      <c r="D72" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D72" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E72" t="s">
         <v>8</v>
@@ -2161,7 +2169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>81</v>
       </c>
@@ -2171,8 +2179,8 @@
       <c r="C73" s="1">
         <v>45911</v>
       </c>
-      <c r="D73" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D73" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E73" t="s">
         <v>8</v>
@@ -2181,7 +2189,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>82</v>
       </c>
@@ -2191,8 +2199,8 @@
       <c r="C74" s="1">
         <v>45911</v>
       </c>
-      <c r="D74" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D74" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E74" t="s">
         <v>8</v>
@@ -2201,7 +2209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>83</v>
       </c>
@@ -2211,8 +2219,8 @@
       <c r="C75" s="1">
         <v>45911</v>
       </c>
-      <c r="D75" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D75" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E75" t="s">
         <v>8</v>
@@ -2221,7 +2229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -2231,8 +2239,8 @@
       <c r="C76" s="1">
         <v>45911</v>
       </c>
-      <c r="D76" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D76" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E76" t="s">
         <v>8</v>
@@ -2241,7 +2249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>85</v>
       </c>
@@ -2251,8 +2259,8 @@
       <c r="C77" s="1">
         <v>45911</v>
       </c>
-      <c r="D77" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D77" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E77" t="s">
         <v>8</v>
@@ -2261,7 +2269,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>86</v>
       </c>
@@ -2271,8 +2279,8 @@
       <c r="C78" s="1">
         <v>45911</v>
       </c>
-      <c r="D78" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D78" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E78" t="s">
         <v>12</v>
@@ -2281,7 +2289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>87</v>
       </c>
@@ -2291,8 +2299,8 @@
       <c r="C79" s="1">
         <v>45911</v>
       </c>
-      <c r="D79" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D79" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E79" t="s">
         <v>8</v>
@@ -2301,7 +2309,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>88</v>
       </c>
@@ -2311,8 +2319,8 @@
       <c r="C80" s="1">
         <v>45911</v>
       </c>
-      <c r="D80" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D80" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E80" t="s">
         <v>8</v>
@@ -2321,7 +2329,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>89</v>
       </c>
@@ -2331,8 +2339,8 @@
       <c r="C81" s="1">
         <v>45911</v>
       </c>
-      <c r="D81" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D81" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E81" t="s">
         <v>8</v>
@@ -2341,7 +2349,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -2351,8 +2359,8 @@
       <c r="C82" s="1">
         <v>45911</v>
       </c>
-      <c r="D82" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D82" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E82" t="s">
         <v>8</v>
@@ -2361,7 +2369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>91</v>
       </c>
@@ -2371,8 +2379,8 @@
       <c r="C83" s="1">
         <v>45911</v>
       </c>
-      <c r="D83" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D83" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E83" t="s">
         <v>8</v>
@@ -2381,7 +2389,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -2391,8 +2399,8 @@
       <c r="C84" s="1">
         <v>45911</v>
       </c>
-      <c r="D84" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D84" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
@@ -2401,7 +2409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>93</v>
       </c>
@@ -2411,8 +2419,8 @@
       <c r="C85" s="1">
         <v>45911</v>
       </c>
-      <c r="D85" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D85" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
@@ -2421,7 +2429,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>94</v>
       </c>
@@ -2431,8 +2439,8 @@
       <c r="C86" s="1">
         <v>45911</v>
       </c>
-      <c r="D86" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D86" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E86" t="s">
         <v>12</v>
@@ -2441,7 +2449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>95</v>
       </c>
@@ -2451,8 +2459,8 @@
       <c r="C87" s="1">
         <v>45911</v>
       </c>
-      <c r="D87" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D87" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E87" t="s">
         <v>8</v>
@@ -2461,7 +2469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>96</v>
       </c>
@@ -2471,8 +2479,8 @@
       <c r="C88" s="1">
         <v>45911</v>
       </c>
-      <c r="D88" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D88" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E88" t="s">
         <v>8</v>
@@ -2481,7 +2489,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>97</v>
       </c>
@@ -2491,8 +2499,8 @@
       <c r="C89" s="1">
         <v>45911</v>
       </c>
-      <c r="D89" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D89" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E89" t="s">
         <v>8</v>
@@ -2501,7 +2509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>98</v>
       </c>
@@ -2511,8 +2519,8 @@
       <c r="C90" s="1">
         <v>45911</v>
       </c>
-      <c r="D90" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D90" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E90" t="s">
         <v>12</v>
@@ -2521,7 +2529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>99</v>
       </c>
@@ -2531,8 +2539,8 @@
       <c r="C91" s="1">
         <v>45911</v>
       </c>
-      <c r="D91" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D91" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E91" t="s">
         <v>8</v>
@@ -2541,7 +2549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>100</v>
       </c>
@@ -2551,8 +2559,8 @@
       <c r="C92" s="1">
         <v>45911</v>
       </c>
-      <c r="D92" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D92" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E92" t="s">
         <v>8</v>
@@ -2561,7 +2569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>101</v>
       </c>
@@ -2571,8 +2579,8 @@
       <c r="C93" s="1">
         <v>45911</v>
       </c>
-      <c r="D93" s="2">
-        <v>0.47916666666666669</v>
+      <c r="D93" s="3">
+        <v>0.460590277777778</v>
       </c>
       <c r="E93" t="s">
         <v>8</v>

</xml_diff>